<commit_message>
Added in pop-pyrmaids to Graphics dir, pasted ZALCM and ZAHMI pop pyramids to BPs
</commit_message>
<xml_diff>
--- a/reports/pop_age_pyramid.xlsx
+++ b/reports/pop_age_pyramid.xlsx
@@ -3438,8 +3438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>

</xml_diff>